<commit_message>
Ajustando Obtenção de Constantes
</commit_message>
<xml_diff>
--- a/tests/testthat/Dados_Template_Fonte_Dados.xlsx
+++ b/tests/testthat/Dados_Template_Fonte_Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7470" tabRatio="749" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constantes" sheetId="36" r:id="rId1"/>
@@ -39,7 +39,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Cenarios!$A$1:$C$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$A$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Constantes!$A$1:$A$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">Custos!$A$1:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Eventos_Inic!$A$2:$L$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">Funcoes_Inputs!$A$1:$I$226</definedName>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3006" uniqueCount="563">
   <si>
     <t>Ano</t>
   </si>
@@ -2750,9 +2750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D83D282-F75C-4952-B6E5-FA904FFBD51F}">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2800,246 +2802,231 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="83" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="83" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="83" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="83" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="83" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="83" t="s">
-        <v>95</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="83" t="s">
-        <v>126</v>
+        <v>466</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="83" t="s">
-        <v>132</v>
+        <v>468</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="83" t="s">
-        <v>142</v>
+        <v>538</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="83" t="s">
-        <v>466</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>468</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="83" t="s">
-        <v>538</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="83" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="83" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="83" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="83" t="s">
-        <v>151</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="83" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="83" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="83" t="s">
-        <v>200</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="83" t="s">
-        <v>201</v>
+      <c r="A32" s="93" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="83" t="s">
-        <v>202</v>
+      <c r="A33" s="93" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="93" t="s">
-        <v>144</v>
+      <c r="A35" s="83" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="93" t="s">
-        <v>145</v>
+      <c r="A36" s="83" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="83" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="83" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>161</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="83" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="83" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="83" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="83" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="83" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
-        <v>206</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="83" t="s">
-        <v>207</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="83" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="83" t="s">
-        <v>125</v>
+        <v>461</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
-        <v>123</v>
+        <v>462</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="83" t="s">
-        <v>124</v>
+        <v>463</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="83" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="83" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="83" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="83" t="s">
         <v>464</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A55" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
+  <autoFilter ref="A1:A52" xr:uid="{E72623EE-AF76-4665-8E1C-61480EAE2A81}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -22995,9 +22982,9 @@
   </sheetPr>
   <dimension ref="A1:P157"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F155" sqref="F155"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>